<commit_message>
modelo base de datos
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencia documentacion/Fase de Testing.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencia documentacion/Fase de Testing.xlsx
@@ -16,9 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Fase de testing</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+  <si>
+    <t>Fase de testing (Pre-mitigacion)</t>
+  </si>
+  <si>
+    <t>Fase de testing (Post-mitigacion)</t>
+  </si>
+  <si>
+    <t>Comentarios de mitigacion</t>
   </si>
   <si>
     <t>Requerimientos Faltantes</t>
@@ -27,6 +33,9 @@
     <t>Boton Home desde todas las pestañas</t>
   </si>
   <si>
+    <t>Error ya mitigado</t>
+  </si>
+  <si>
     <t>Enalazar Pestaña "Mis datos"</t>
   </si>
   <si>
@@ -36,49 +45,91 @@
     <t>Hacer la pagina mas responsiva</t>
   </si>
   <si>
+    <t>Todas las paginas del proyecto estan responsivas en caso de acceder desde el celular</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eliminar enlaze de  pestaña de capacitaciones en  el panel para usuarios no requeridos (o enlazarla) </t>
   </si>
   <si>
+    <t xml:space="preserve">Advertensia eliminada correctamente </t>
+  </si>
+  <si>
     <t>Boton de cerrar sesion abajo del panel no funciona</t>
   </si>
   <si>
+    <t>Se elimino la funionalidad de errar sesion del panel que no hacia nada</t>
+  </si>
+  <si>
     <t>Enlazar documentos</t>
   </si>
   <si>
+    <t>se enlazo correctamente</t>
+  </si>
+  <si>
     <t>Enlazar foro</t>
   </si>
   <si>
     <t>desde ka pestaña de solicitudes.php solicitudes de usuario en el panel no funciona</t>
   </si>
   <si>
+    <t>Habia un pequeño error en la importacion del archivo .js</t>
+  </si>
+  <si>
     <t>filtro de sooporte de informatico en soporte_def.php se cae</t>
   </si>
   <si>
+    <t>Ya se soluciono para que filtre por ambos (estado y area)</t>
+  </si>
+  <si>
     <t>al abrir el panel no se sobrepone a lo que hay en pantalla y desordena la pagina</t>
   </si>
   <si>
+    <t>Ya se soluciono correctamente</t>
+  </si>
+  <si>
     <t>Boton de buscar en la parte superior de home no hace nada</t>
   </si>
   <si>
+    <t>Se quito boton ya qu eno es necesario al poseer pocas paginas</t>
+  </si>
+  <si>
     <t>el rut del usuario sale dos veces en la parte superior</t>
   </si>
   <si>
+    <t>Aclaracion, uno es la ficha y el otro es el rut</t>
+  </si>
+  <si>
     <t>En el panel las pestañas bajan pero no regresan a su sitio correspondiente</t>
   </si>
   <si>
+    <t>se soluciono completamente, habia un pequeño error al cerrar un div</t>
+  </si>
+  <si>
     <t>Motrar nombre de los iconos en el panel lateral (Capacitaciones, encuestas, documentos. Foro)</t>
   </si>
   <si>
+    <t>See muestran correctamente los nombres</t>
+  </si>
+  <si>
     <t>Enlazar solicitudes de usuario</t>
   </si>
   <si>
     <t>en respuesta a encuesta, el detalle se muestra pero no se puede encoger a menos que selecciones otro</t>
   </si>
   <si>
+    <t>Ahora si se pueden econger</t>
+  </si>
+  <si>
     <t>enlazar agregar empleado mes</t>
   </si>
   <si>
+    <t>enlazdo correctamente</t>
+  </si>
+  <si>
     <t>desde la vistra de rrhh los usuarios nuevos se ven mal en pantallas muy grandes</t>
+  </si>
+  <si>
+    <t>ya se soluciono el % de vh del usuario</t>
   </si>
 </sst>
 </file>
@@ -122,20 +173,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8ED873"/>
-        <bgColor rgb="FF8ED873"/>
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
   </fills>
@@ -151,35 +202,50 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -399,151 +465,288 @@
     <col customWidth="1" min="1" max="1" width="10.63"/>
     <col customWidth="1" min="2" max="2" width="37.63"/>
     <col customWidth="1" min="3" max="3" width="45.13"/>
-    <col customWidth="1" min="4" max="26" width="10.63"/>
+    <col customWidth="1" min="4" max="5" width="39.88"/>
+    <col customWidth="1" min="6" max="26" width="10.63"/>
   </cols>
   <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="6">
-      <c r="B6" s="1" t="s">
-        <v>0</v>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3"/>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8">
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9">
-      <c r="B9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3"/>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11">
-      <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3"/>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12">
-      <c r="B12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3"/>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13">
-      <c r="B13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3"/>
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14">
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="3"/>
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
-      <c r="B16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17">
-      <c r="B17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="3"/>
+      <c r="B17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18">
-      <c r="B18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="3"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
     </row>
     <row r="19">
-      <c r="B19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="3"/>
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="3"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="3"/>
+      <c r="B24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="3"/>
+      <c r="B26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="3"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1"/>

</xml_diff>